<commit_message>
updates to pull data and fixes
</commit_message>
<xml_diff>
--- a/Liquidity/Global_M2/Datasums/long27_DataComp.xlsx
+++ b/Liquidity/Global_M2/Datasums/long27_DataComp.xlsx
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D2" t="n">
         <v>500</v>
@@ -515,13 +515,13 @@
         <v>35065</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -555,10 +555,10 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" s="2" t="n">
-        <v>30529</v>
+        <v>30376</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45717</v>
+        <v>45566</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -596,16 +596,16 @@
         <v>500</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>30529</v>
+        <v>30348</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -641,16 +641,16 @@
         <v>500</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>30560</v>
+        <v>30376</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45748</v>
+        <v>45566</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D6" t="n">
         <v>500</v>
@@ -689,13 +689,13 @@
         <v>31747</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -731,16 +731,16 @@
         <v>500</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>30498</v>
+        <v>30348</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45689</v>
+        <v>45536</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -773,19 +773,19 @@
         <v>500</v>
       </c>
       <c r="D8" t="n">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>30529</v>
+        <v>30348</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -821,16 +821,16 @@
         <v>500</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>30529</v>
+        <v>30348</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -863,19 +863,19 @@
         <v>500</v>
       </c>
       <c r="D10" t="n">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>30529</v>
+        <v>30376</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45717</v>
+        <v>45566</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>30592</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -911,16 +911,16 @@
         <v>500</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>30498</v>
+        <v>30348</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45689</v>
+        <v>45536</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -950,22 +950,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D12" t="n">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>33939</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>34578</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D13" t="n">
         <v>500</v>
@@ -1004,13 +1004,13 @@
         <v>31017</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>45717</v>
+        <v>45566</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1040,22 +1040,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D14" t="n">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>32325</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>33239</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D15" t="n">
         <v>500</v>
@@ -1094,13 +1094,13 @@
         <v>33543</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>45689</v>
+        <v>45536</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>30560</v>
+        <v>30376</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1130,22 +1130,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D16" t="n">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>31382</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>45717</v>
+        <v>45505</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1175,22 +1175,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D17" t="n">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>33970</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>33298</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1223,19 +1223,19 @@
         <v>500</v>
       </c>
       <c r="D18" t="n">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>30529</v>
+        <v>30348</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>37377</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1268,19 +1268,19 @@
         <v>500</v>
       </c>
       <c r="D19" t="n">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>30529</v>
+        <v>30376</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>45717</v>
+        <v>45566</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>33178</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="D20" t="n">
         <v>500</v>
@@ -1319,13 +1319,13 @@
         <v>25903</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1361,16 +1361,16 @@
         <v>500</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>30529</v>
+        <v>30376</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>45717</v>
+        <v>45566</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1403,19 +1403,19 @@
         <v>500</v>
       </c>
       <c r="D22" t="n">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>30529</v>
+        <v>30348</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>33725</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1448,19 +1448,19 @@
         <v>500</v>
       </c>
       <c r="D23" t="n">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>30529</v>
+        <v>30348</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>35339</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D24" t="n">
         <v>500</v>
@@ -1499,13 +1499,13 @@
         <v>33239</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1541,16 +1541,16 @@
         <v>500</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>30529</v>
+        <v>30348</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>30592</v>
+        <v>30407</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1580,22 +1580,22 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D26" t="n">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>31413</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>45748</v>
+        <v>45536</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>33178</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1628,19 +1628,19 @@
         <v>500</v>
       </c>
       <c r="D27" t="n">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>30529</v>
+        <v>30376</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>45717</v>
+        <v>45566</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1670,22 +1670,22 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D28" t="n">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>34304</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>45717</v>
+        <v>45566</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>34121</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>45778</v>
+        <v>45597</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>

</xml_diff>